<commit_message>
temp wire and add print statements to check, may require delay
</commit_message>
<xml_diff>
--- a/wiring.xlsx
+++ b/wiring.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@Sumobot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sumobot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B805AD8-5C80-44A1-82BC-D3BEAB83B830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421D6A14-704F-4958-BF76-DC88A0841860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,7 +381,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>